<commit_message>
coverted the project in testng and divided into groups smoke,sanity and regression
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/TestData.xlsx
+++ b/src/test/resources/TestData/TestData.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="92">
   <si>
     <t>TestCases</t>
   </si>
@@ -294,6 +294,12 @@
   </si>
   <si>
     <t>bandar@123</t>
+  </si>
+  <si>
+    <t>nonu@gm.com</t>
+  </si>
+  <si>
+    <t>bm@123</t>
   </si>
 </sst>
 </file>
@@ -1021,10 +1027,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1052,9 +1058,21 @@
         <v>89</v>
       </c>
     </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>91</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A3" r:id="rId1"/>
+    <hyperlink ref="B3" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId3"/>
 </worksheet>
 </file>
 

</xml_diff>